<commit_message>
fix array vs single, update docs
</commit_message>
<xml_diff>
--- a/props_table.xlsx
+++ b/props_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\svg-simple-draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD08B116-AA6B-49DC-9562-F1A4D16D0B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF0AFE8-474E-4EB7-A41A-99EDAF3FCBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2C2840-DFCF-4DE3-A1EE-66D0B1986D31}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>fill</t>
   </si>
@@ -56,18 +56,12 @@
     <t>```'inherit'```</t>
   </si>
   <si>
-    <t>```fill: "red"```</t>
-  </si>
-  <si>
     <t>stroke</t>
   </si>
   <si>
     <t>The stroke color for the SVG</t>
   </si>
   <si>
-    <t>```stroke: "red"```</t>
-  </si>
-  <si>
     <t>Accepts</t>
   </si>
   <si>
@@ -80,18 +74,12 @@
     <t>The width of the SVG stroke</t>
   </si>
   <si>
-    <t>```strokeWidth: "20px"```</t>
-  </si>
-  <si>
     <t>fillOpacity</t>
   </si>
   <si>
     <t>The opacity of the SVG fill</t>
   </si>
   <si>
-    <t>```fillOpacity: 0.2```</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -101,45 +89,24 @@
     <t>SVG width</t>
   </si>
   <si>
-    <t>string|number</t>
-  </si>
-  <si>
     <t>height</t>
   </si>
   <si>
     <t>SVG height</t>
   </si>
   <si>
-    <t>```width: "20px"```</t>
-  </si>
-  <si>
-    <t>```height: "20px"```</t>
-  </si>
-  <si>
     <t>animation</t>
   </si>
   <si>
-    <t>The name of the animation desired, if only one is desired</t>
-  </si>
-  <si>
     <t>```'none'```</t>
   </si>
   <si>
-    <t>```'fade-in-stroke'```</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
-    <t>The duration of the animation desired, if only one is desired</t>
-  </si>
-  <si>
     <t>```'0.5s'```</t>
   </si>
   <si>
-    <t>```'2.5s'```</t>
-  </si>
-  <si>
     <t>animationNames</t>
   </si>
   <si>
@@ -152,9 +119,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>```['fade-in-fill', 'fade-in-stroke']```</t>
-  </si>
-  <si>
     <t>animationDurations</t>
   </si>
   <si>
@@ -164,7 +128,91 @@
     <t>null (if animation name is present without duration, defaults to '0.5s')</t>
   </si>
   <si>
-    <t>```['0.5s', '3s']```</t>
+    <t>animationIterationCounts</t>
+  </si>
+  <si>
+    <t>An array of animation iteration counts (maps 1 to 1 to animation names)</t>
+  </si>
+  <si>
+    <t>null (if animation name is present without duration, defaults to '1')</t>
+  </si>
+  <si>
+    <t>animationTimingFunctions</t>
+  </si>
+  <si>
+    <t>An array of animation timing functions (maps 1 to 1 to animation names)</t>
+  </si>
+  <si>
+    <t>null (if animation name is present without duration, defaults to none)</t>
+  </si>
+  <si>
+    <t>```1```</t>
+  </si>
+  <si>
+    <t>The desired iteration count, if only one animation in use</t>
+  </si>
+  <si>
+    <t>The duration of the animation desired, if only one animation in use</t>
+  </si>
+  <si>
+    <t>The name of the animation desired, if only one animation in use</t>
+  </si>
+  <si>
+    <t>The desired timing function, if only one animation in use</t>
+  </si>
+  <si>
+    <t>iterationCount</t>
+  </si>
+  <si>
+    <t>timingFunction</t>
+  </si>
+  <si>
+    <t>```width="20px"```</t>
+  </si>
+  <si>
+    <t>```strokeWidth="20px"```</t>
+  </si>
+  <si>
+    <t>```stroke="red"```</t>
+  </si>
+  <si>
+    <t>```fill="red"```</t>
+  </si>
+  <si>
+    <t>```duration='2.5s'```</t>
+  </si>
+  <si>
+    <t>```animation='fade-in-stroke'```</t>
+  </si>
+  <si>
+    <t>```height="20px"```</t>
+  </si>
+  <si>
+    <t>```fillOpacity={0.2}```</t>
+  </si>
+  <si>
+    <t>```iterationCount='infinite'```</t>
+  </si>
+  <si>
+    <t>```timingFunction='linear'```</t>
+  </si>
+  <si>
+    <t>```animationNames={['fade-in-fill', 'fade-in-stroke']}```</t>
+  </si>
+  <si>
+    <t>```animationDurations={['0.5s', '3s']}```</t>
+  </si>
+  <si>
+    <t>```animationIterationCounts={['infinite','',3]}```</t>
+  </si>
+  <si>
+    <t>```animationTimingFunctions={['linear','','']}```</t>
+  </si>
+  <si>
+    <t>string or number</t>
+  </si>
+  <si>
+    <t>string ornumber</t>
   </si>
 </sst>
 </file>
@@ -516,13 +564,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE096B3-AEB0-4AA3-8F97-5FD498B09D90}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -532,7 +587,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -549,169 +604,238 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>